<commit_message>
Add Mark for each question
</commit_message>
<xml_diff>
--- a/NamelistAndAnswerTemplate.xlsx
+++ b/NamelistAndAnswerTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\cyrus\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CEAF7612-4955-4E19-ABFB-F3F5F69047F2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BC8EB3F-CF95-4B6F-9D5A-603C023726D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1425" windowWidth="29040" windowHeight="15840" xr2:uid="{A1884D39-ABA1-4617-A172-367CF3293095}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{A1884D39-ABA1-4617-A172-367CF3293095}"/>
   </bookViews>
   <sheets>
     <sheet name="Answer" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Question</t>
   </si>
@@ -64,6 +64,9 @@
   </si>
   <si>
     <t>StudentID</t>
+  </si>
+  <si>
+    <t>Mark</t>
   </si>
 </sst>
 </file>
@@ -415,10 +418,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8EC2EE06-8B09-480F-9E9A-B802BB94EF83}">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B5"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -426,30 +429,33 @@
     <col min="2" max="2" width="11.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>5</v>
       </c>

</xml_diff>